<commit_message>
add Platan and Bonaerian
</commit_message>
<xml_diff>
--- a/data_2023/time_bins/SALMA.xlsx
+++ b/data_2023/time_bins/SALMA.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\Internship_ISEM\Neotropical_Mammals\REPO\Neotropical_mammals\data_2023\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\Internship_ISEM\Neotropical_Mammals\REPO\Neotropical_mammals\data_2023\time_bins\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7A93A10C-300C-45A1-939D-4F2CB0009865}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EA6F7A98-FBCA-48D6-8A63-54F6B975326B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="768" yWindow="768" windowWidth="17280" windowHeight="8880" xr2:uid="{04C64777-6055-495D-8002-BBD1BCB13666}"/>
+    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="17520" xr2:uid="{04C64777-6055-495D-8002-BBD1BCB13666}"/>
   </bookViews>
   <sheets>
     <sheet name="Feuil1" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="50" uniqueCount="33">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="54" uniqueCount="36">
   <si>
     <t>min_ma</t>
   </si>
@@ -142,6 +142,15 @@
   </si>
   <si>
     <t>interval_name</t>
+  </si>
+  <si>
+    <t>Bonaerian</t>
+  </si>
+  <si>
+    <t>Holocene</t>
+  </si>
+  <si>
+    <t>Platan</t>
   </si>
 </sst>
 </file>
@@ -521,10 +530,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{050431C4-1A0C-4966-AE29-90D56A8311BE}">
-  <dimension ref="A1:D24"/>
+  <dimension ref="A1:D26"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B2" sqref="B2"/>
+      <selection activeCell="D3" sqref="D3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -548,16 +557,16 @@
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A2" s="2" t="s">
-        <v>3</v>
+        <v>34</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>2</v>
+        <v>35</v>
       </c>
       <c r="C2" s="2">
         <v>0</v>
       </c>
       <c r="D2" s="2">
-        <v>1</v>
+        <v>1.17E-2</v>
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.3">
@@ -565,41 +574,41 @@
         <v>3</v>
       </c>
       <c r="B3" s="2" t="s">
-        <v>6</v>
+        <v>2</v>
       </c>
       <c r="C3" s="2">
-        <v>1</v>
+        <v>1.17E-2</v>
       </c>
       <c r="D3" s="2">
-        <v>2</v>
+        <v>0.3</v>
       </c>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A4" s="2" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="B4" s="2" t="s">
-        <v>26</v>
+        <v>33</v>
       </c>
       <c r="C4" s="2">
-        <v>2</v>
+        <v>0.3</v>
       </c>
       <c r="D4" s="2">
-        <v>3</v>
+        <v>0.7</v>
       </c>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A5" s="2" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="B5" s="2" t="s">
-        <v>28</v>
+        <v>6</v>
       </c>
       <c r="C5" s="2">
-        <v>3</v>
+        <v>0.7</v>
       </c>
       <c r="D5" s="2">
-        <v>4</v>
+        <v>2</v>
       </c>
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.3">
@@ -607,41 +616,41 @@
         <v>4</v>
       </c>
       <c r="B6" s="2" t="s">
-        <v>7</v>
+        <v>26</v>
       </c>
       <c r="C6" s="2">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="D6" s="2">
-        <v>5.3330000000000002</v>
+        <v>3</v>
       </c>
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A7" s="2" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="B7" s="2" t="s">
-        <v>8</v>
+        <v>28</v>
       </c>
       <c r="C7" s="2">
-        <v>5.3330000000000002</v>
+        <v>3</v>
       </c>
       <c r="D7" s="2">
-        <v>8</v>
+        <v>4</v>
       </c>
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A8" s="2" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="B8" s="2" t="s">
-        <v>9</v>
+        <v>7</v>
       </c>
       <c r="C8" s="2">
-        <v>8</v>
+        <v>4</v>
       </c>
       <c r="D8" s="2">
-        <v>9</v>
+        <v>5.3330000000000002</v>
       </c>
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.3">
@@ -649,13 +658,13 @@
         <v>5</v>
       </c>
       <c r="B9" s="2" t="s">
-        <v>29</v>
+        <v>8</v>
       </c>
       <c r="C9" s="2">
-        <v>10</v>
+        <v>5.3330000000000002</v>
       </c>
       <c r="D9" s="2">
-        <v>11.5</v>
+        <v>8</v>
       </c>
     </row>
     <row r="10" spans="1:4" x14ac:dyDescent="0.3">
@@ -663,13 +672,13 @@
         <v>5</v>
       </c>
       <c r="B10" s="2" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="C10" s="2">
-        <v>11.5</v>
+        <v>8</v>
       </c>
       <c r="D10" s="2">
-        <v>13</v>
+        <v>9</v>
       </c>
     </row>
     <row r="11" spans="1:4" x14ac:dyDescent="0.3">
@@ -677,13 +686,13 @@
         <v>5</v>
       </c>
       <c r="B11" s="2" t="s">
-        <v>11</v>
+        <v>29</v>
       </c>
       <c r="C11" s="2">
-        <v>14</v>
+        <v>10</v>
       </c>
       <c r="D11" s="2">
-        <v>15</v>
+        <v>11.5</v>
       </c>
     </row>
     <row r="12" spans="1:4" x14ac:dyDescent="0.3">
@@ -691,13 +700,13 @@
         <v>5</v>
       </c>
       <c r="B12" s="2" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="C12" s="2">
-        <v>16</v>
+        <v>11.5</v>
       </c>
       <c r="D12" s="2">
-        <v>18</v>
+        <v>13</v>
       </c>
     </row>
     <row r="13" spans="1:4" x14ac:dyDescent="0.3">
@@ -705,69 +714,69 @@
         <v>5</v>
       </c>
       <c r="B13" s="2" t="s">
-        <v>25</v>
+        <v>11</v>
       </c>
       <c r="C13" s="2">
-        <v>20</v>
+        <v>14</v>
       </c>
       <c r="D13" s="2">
-        <v>21</v>
+        <v>15</v>
       </c>
     </row>
     <row r="14" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A14" s="2" t="s">
-        <v>13</v>
+        <v>5</v>
       </c>
       <c r="B14" s="2" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
       <c r="C14" s="2">
-        <v>23.03</v>
+        <v>16</v>
       </c>
       <c r="D14" s="2">
-        <v>30</v>
+        <v>18</v>
       </c>
     </row>
     <row r="15" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A15" s="2" t="s">
-        <v>13</v>
+        <v>5</v>
       </c>
       <c r="B15" s="2" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
       <c r="C15" s="2">
-        <v>30</v>
+        <v>20</v>
       </c>
       <c r="D15" s="2">
-        <v>33.9</v>
+        <v>21</v>
       </c>
     </row>
     <row r="16" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A16" s="2" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="B16" s="2" t="s">
-        <v>16</v>
+        <v>14</v>
       </c>
       <c r="C16" s="2">
-        <v>36</v>
+        <v>23.03</v>
       </c>
       <c r="D16" s="2">
-        <v>39</v>
+        <v>30</v>
       </c>
     </row>
     <row r="17" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A17" s="2" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="B17" s="2" t="s">
-        <v>17</v>
+        <v>27</v>
       </c>
       <c r="C17" s="2">
-        <v>39.5</v>
+        <v>30</v>
       </c>
       <c r="D17" s="2">
-        <v>42</v>
+        <v>33.9</v>
       </c>
     </row>
     <row r="18" spans="1:4" x14ac:dyDescent="0.3">
@@ -775,13 +784,13 @@
         <v>15</v>
       </c>
       <c r="B18" s="2" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="C18" s="2">
-        <v>44</v>
+        <v>36</v>
       </c>
       <c r="D18" s="2">
-        <v>45</v>
+        <v>39</v>
       </c>
     </row>
     <row r="19" spans="1:4" x14ac:dyDescent="0.3">
@@ -789,13 +798,13 @@
         <v>15</v>
       </c>
       <c r="B19" s="2" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="C19" s="2">
-        <v>47</v>
+        <v>39.5</v>
       </c>
       <c r="D19" s="2">
-        <v>48</v>
+        <v>42</v>
       </c>
     </row>
     <row r="20" spans="1:4" x14ac:dyDescent="0.3">
@@ -803,13 +812,13 @@
         <v>15</v>
       </c>
       <c r="B20" s="2" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
       <c r="C20" s="2">
-        <v>50</v>
+        <v>44</v>
       </c>
       <c r="D20" s="2">
-        <v>51</v>
+        <v>45</v>
       </c>
     </row>
     <row r="21" spans="1:4" x14ac:dyDescent="0.3">
@@ -817,41 +826,41 @@
         <v>15</v>
       </c>
       <c r="B21" s="2" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="C21" s="2">
-        <v>51</v>
+        <v>47</v>
       </c>
       <c r="D21" s="2">
-        <v>56</v>
+        <v>48</v>
       </c>
     </row>
     <row r="22" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A22" s="2" t="s">
-        <v>22</v>
+        <v>15</v>
       </c>
       <c r="B22" s="2" t="s">
-        <v>30</v>
+        <v>20</v>
       </c>
       <c r="C22" s="2">
-        <v>59.2</v>
+        <v>50</v>
       </c>
       <c r="D22" s="2">
-        <v>61</v>
+        <v>51</v>
       </c>
     </row>
     <row r="23" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A23" s="2" t="s">
-        <v>22</v>
+        <v>15</v>
       </c>
       <c r="B23" s="2" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
       <c r="C23" s="2">
-        <v>62</v>
+        <v>51</v>
       </c>
       <c r="D23" s="2">
-        <v>63</v>
+        <v>56</v>
       </c>
     </row>
     <row r="24" spans="1:4" x14ac:dyDescent="0.3">
@@ -859,12 +868,40 @@
         <v>22</v>
       </c>
       <c r="B24" s="2" t="s">
+        <v>30</v>
+      </c>
+      <c r="C24" s="2">
+        <v>59.2</v>
+      </c>
+      <c r="D24" s="2">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="25" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A25" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="B25" s="2" t="s">
+        <v>23</v>
+      </c>
+      <c r="C25" s="2">
+        <v>62</v>
+      </c>
+      <c r="D25" s="2">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="26" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A26" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="B26" s="2" t="s">
         <v>24</v>
       </c>
-      <c r="C24" s="2">
+      <c r="C26" s="2">
         <v>64</v>
       </c>
-      <c r="D24" s="2">
+      <c r="D26" s="2">
         <v>66</v>
       </c>
     </row>

</xml_diff>

<commit_message>
add Friasian and Casamayoran
</commit_message>
<xml_diff>
--- a/data_2023/time_bins/SALMA.xlsx
+++ b/data_2023/time_bins/SALMA.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\Internship_ISEM\Neotropical_Mammals\REPO\Neotropical_mammals\data_2023\time_bins\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EA6F7A98-FBCA-48D6-8A63-54F6B975326B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{35B06040-8C6E-494F-AB55-B6D328B32547}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="17520" xr2:uid="{04C64777-6055-495D-8002-BBD1BCB13666}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="54" uniqueCount="36">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="58" uniqueCount="38">
   <si>
     <t>min_ma</t>
   </si>
@@ -151,6 +151,12 @@
   </si>
   <si>
     <t>Platan</t>
+  </si>
+  <si>
+    <t>Casamayoran</t>
+  </si>
+  <si>
+    <t>Friasian</t>
   </si>
 </sst>
 </file>
@@ -530,10 +536,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{050431C4-1A0C-4966-AE29-90D56A8311BE}">
-  <dimension ref="A1:D26"/>
+  <dimension ref="A1:D28"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D3" sqref="D3"/>
+      <selection activeCell="A14" sqref="A14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -720,7 +726,7 @@
         <v>14</v>
       </c>
       <c r="D13" s="2">
-        <v>15</v>
+        <v>15.5</v>
       </c>
     </row>
     <row r="14" spans="1:4" x14ac:dyDescent="0.3">
@@ -728,13 +734,13 @@
         <v>5</v>
       </c>
       <c r="B14" s="2" t="s">
-        <v>12</v>
+        <v>37</v>
       </c>
       <c r="C14" s="2">
-        <v>16</v>
+        <v>15.5</v>
       </c>
       <c r="D14" s="2">
-        <v>18</v>
+        <v>16.3</v>
       </c>
     </row>
     <row r="15" spans="1:4" x14ac:dyDescent="0.3">
@@ -742,27 +748,27 @@
         <v>5</v>
       </c>
       <c r="B15" s="2" t="s">
-        <v>25</v>
+        <v>12</v>
       </c>
       <c r="C15" s="2">
-        <v>20</v>
+        <v>16.3</v>
       </c>
       <c r="D15" s="2">
-        <v>21</v>
+        <v>18</v>
       </c>
     </row>
     <row r="16" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A16" s="2" t="s">
-        <v>13</v>
+        <v>5</v>
       </c>
       <c r="B16" s="2" t="s">
-        <v>14</v>
+        <v>25</v>
       </c>
       <c r="C16" s="2">
-        <v>23.03</v>
+        <v>20</v>
       </c>
       <c r="D16" s="2">
-        <v>30</v>
+        <v>21</v>
       </c>
     </row>
     <row r="17" spans="1:4" x14ac:dyDescent="0.3">
@@ -770,27 +776,27 @@
         <v>13</v>
       </c>
       <c r="B17" s="2" t="s">
-        <v>27</v>
+        <v>14</v>
       </c>
       <c r="C17" s="2">
+        <v>23.03</v>
+      </c>
+      <c r="D17" s="2">
         <v>30</v>
-      </c>
-      <c r="D17" s="2">
-        <v>33.9</v>
       </c>
     </row>
     <row r="18" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A18" s="2" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="B18" s="2" t="s">
-        <v>16</v>
+        <v>27</v>
       </c>
       <c r="C18" s="2">
-        <v>36</v>
+        <v>30</v>
       </c>
       <c r="D18" s="2">
-        <v>39</v>
+        <v>33.9</v>
       </c>
     </row>
     <row r="19" spans="1:4" x14ac:dyDescent="0.3">
@@ -798,13 +804,13 @@
         <v>15</v>
       </c>
       <c r="B19" s="2" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="C19" s="2">
-        <v>39.5</v>
+        <v>36</v>
       </c>
       <c r="D19" s="2">
-        <v>42</v>
+        <v>39</v>
       </c>
     </row>
     <row r="20" spans="1:4" x14ac:dyDescent="0.3">
@@ -812,13 +818,13 @@
         <v>15</v>
       </c>
       <c r="B20" s="2" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="C20" s="2">
-        <v>44</v>
+        <v>39.5</v>
       </c>
       <c r="D20" s="2">
-        <v>45</v>
+        <v>42</v>
       </c>
     </row>
     <row r="21" spans="1:4" x14ac:dyDescent="0.3">
@@ -826,13 +832,13 @@
         <v>15</v>
       </c>
       <c r="B21" s="2" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="C21" s="2">
-        <v>47</v>
+        <v>44</v>
       </c>
       <c r="D21" s="2">
-        <v>48</v>
+        <v>45</v>
       </c>
     </row>
     <row r="22" spans="1:4" x14ac:dyDescent="0.3">
@@ -840,13 +846,13 @@
         <v>15</v>
       </c>
       <c r="B22" s="2" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="C22" s="2">
-        <v>50</v>
+        <v>47</v>
       </c>
       <c r="D22" s="2">
-        <v>51</v>
+        <v>48</v>
       </c>
     </row>
     <row r="23" spans="1:4" x14ac:dyDescent="0.3">
@@ -854,41 +860,41 @@
         <v>15</v>
       </c>
       <c r="B23" s="2" t="s">
-        <v>21</v>
+        <v>36</v>
       </c>
       <c r="C23" s="2">
-        <v>51</v>
+        <v>48</v>
       </c>
       <c r="D23" s="2">
-        <v>56</v>
+        <v>50</v>
       </c>
     </row>
     <row r="24" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A24" s="2" t="s">
-        <v>22</v>
+        <v>15</v>
       </c>
       <c r="B24" s="2" t="s">
-        <v>30</v>
+        <v>20</v>
       </c>
       <c r="C24" s="2">
-        <v>59.2</v>
+        <v>50</v>
       </c>
       <c r="D24" s="2">
-        <v>61</v>
+        <v>51</v>
       </c>
     </row>
     <row r="25" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A25" s="2" t="s">
-        <v>22</v>
+        <v>15</v>
       </c>
       <c r="B25" s="2" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
       <c r="C25" s="2">
-        <v>62</v>
+        <v>51</v>
       </c>
       <c r="D25" s="2">
-        <v>63</v>
+        <v>56</v>
       </c>
     </row>
     <row r="26" spans="1:4" x14ac:dyDescent="0.3">
@@ -896,12 +902,40 @@
         <v>22</v>
       </c>
       <c r="B26" s="2" t="s">
+        <v>30</v>
+      </c>
+      <c r="C26" s="2">
+        <v>59.2</v>
+      </c>
+      <c r="D26" s="2">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="27" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A27" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="B27" s="2" t="s">
+        <v>23</v>
+      </c>
+      <c r="C27" s="2">
+        <v>62</v>
+      </c>
+      <c r="D27" s="2">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="28" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A28" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="B28" s="2" t="s">
         <v>24</v>
       </c>
-      <c r="C26" s="2">
+      <c r="C28" s="2">
         <v>64</v>
       </c>
-      <c r="D26" s="2">
+      <c r="D28" s="2">
         <v>66</v>
       </c>
     </row>

</xml_diff>

<commit_message>
change Laventan upper bound: 13 -> 13.8
And subsequently Colloncuran lower bound: 14 -> 13.8
</commit_message>
<xml_diff>
--- a/data_2023/time_bins/SALMA.xlsx
+++ b/data_2023/time_bins/SALMA.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\Internship_ISEM\Neotropical_Mammals\REPO\Neotropical_mammals\data_2023\time_bins\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CA7E0D02-1414-42AE-B134-2CE152AEAC22}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{25767027-E205-4B89-9BDE-14C20197A037}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="17520" xr2:uid="{04C64777-6055-495D-8002-BBD1BCB13666}"/>
+    <workbookView xWindow="1812" yWindow="1812" windowWidth="17280" windowHeight="8880" xr2:uid="{04C64777-6055-495D-8002-BBD1BCB13666}"/>
   </bookViews>
   <sheets>
     <sheet name="Feuil1" sheetId="1" r:id="rId1"/>
@@ -545,7 +545,7 @@
   <dimension ref="A1:D29"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A6" sqref="A6:XFD6"/>
+      <selection activeCell="C14" sqref="C14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -718,7 +718,7 @@
         <v>11.5</v>
       </c>
       <c r="D12" s="2">
-        <v>13</v>
+        <v>13.8</v>
       </c>
     </row>
     <row r="13" spans="1:4" x14ac:dyDescent="0.3">
@@ -729,7 +729,7 @@
         <v>11</v>
       </c>
       <c r="C13" s="2">
-        <v>14</v>
+        <v>13.8</v>
       </c>
       <c r="D13" s="2">
         <v>15.5</v>

</xml_diff>

<commit_message>
add Gaps to SALMA
</commit_message>
<xml_diff>
--- a/data_2023/time_bins/SALMA.xlsx
+++ b/data_2023/time_bins/SALMA.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\Internship_ISEM\Neotropical_Mammals\REPO\Neotropical_mammals\data_2023\time_bins\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{08E492B0-F40B-4E5D-BC60-EDD5D446EF50}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4A17516E-48F1-4C21-A38E-58778A843042}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="28695" yWindow="0" windowWidth="14610" windowHeight="17385" xr2:uid="{04C64777-6055-495D-8002-BBD1BCB13666}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="56" uniqueCount="38">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="74" uniqueCount="40">
   <si>
     <t>min_ma</t>
   </si>
@@ -168,6 +168,12 @@
   </si>
   <si>
     <t>Pliocene-pleistocene</t>
+  </si>
+  <si>
+    <t>GAP</t>
+  </si>
+  <si>
+    <t>Paleocene-Eocene</t>
   </si>
 </sst>
 </file>
@@ -203,7 +209,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="3">
+  <fills count="4">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -213,6 +219,12 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="2" tint="-0.499984740745262"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFF00"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -229,10 +241,11 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -547,10 +560,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{050431C4-1A0C-4966-AE29-90D56A8311BE}">
-  <dimension ref="A1:D27"/>
+  <dimension ref="A1:D36"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
-      <selection activeCell="E24" sqref="E24"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection sqref="A1:D36"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -769,87 +782,87 @@
       </c>
     </row>
     <row r="16" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A16" s="2" t="s">
+      <c r="A16" s="3" t="s">
         <v>5</v>
       </c>
-      <c r="B16" s="2" t="s">
-        <v>25</v>
-      </c>
-      <c r="C16" s="2">
+      <c r="B16" s="3" t="s">
+        <v>38</v>
+      </c>
+      <c r="C16" s="3">
+        <v>18</v>
+      </c>
+      <c r="D16" s="3">
         <v>20</v>
-      </c>
-      <c r="D16" s="2">
-        <v>21</v>
       </c>
     </row>
     <row r="17" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A17" s="2" t="s">
-        <v>13</v>
+        <v>5</v>
       </c>
       <c r="B17" s="2" t="s">
-        <v>14</v>
+        <v>25</v>
       </c>
       <c r="C17" s="2">
+        <v>20</v>
+      </c>
+      <c r="D17" s="2">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="18" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A18" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="B18" s="3" t="s">
+        <v>38</v>
+      </c>
+      <c r="C18" s="3">
+        <v>21</v>
+      </c>
+      <c r="D18" s="3">
         <v>23.03</v>
-      </c>
-      <c r="D17" s="2">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="18" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A18" s="2" t="s">
-        <v>13</v>
-      </c>
-      <c r="B18" s="2" t="s">
-        <v>27</v>
-      </c>
-      <c r="C18" s="2">
-        <v>30</v>
-      </c>
-      <c r="D18" s="2">
-        <v>33.9</v>
       </c>
     </row>
     <row r="19" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A19" s="2" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="B19" s="2" t="s">
-        <v>16</v>
+        <v>14</v>
       </c>
       <c r="C19" s="2">
-        <v>36</v>
+        <v>23.03</v>
       </c>
       <c r="D19" s="2">
-        <v>39</v>
+        <v>30</v>
       </c>
     </row>
     <row r="20" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A20" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="B20" s="2" t="s">
+        <v>27</v>
+      </c>
+      <c r="C20" s="2">
+        <v>30</v>
+      </c>
+      <c r="D20" s="2">
+        <v>33.9</v>
+      </c>
+    </row>
+    <row r="21" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A21" s="3" t="s">
         <v>15</v>
       </c>
-      <c r="B20" s="2" t="s">
-        <v>17</v>
-      </c>
-      <c r="C20" s="2">
-        <v>39</v>
-      </c>
-      <c r="D20" s="2">
-        <v>42</v>
-      </c>
-    </row>
-    <row r="21" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A21" s="2" t="s">
-        <v>15</v>
-      </c>
-      <c r="B21" s="2" t="s">
-        <v>18</v>
-      </c>
-      <c r="C21" s="2">
-        <v>44</v>
-      </c>
-      <c r="D21" s="2">
-        <v>45</v>
+      <c r="B21" s="3" t="s">
+        <v>38</v>
+      </c>
+      <c r="C21" s="3">
+        <v>33.9</v>
+      </c>
+      <c r="D21" s="3">
+        <v>36</v>
       </c>
     </row>
     <row r="22" spans="1:4" x14ac:dyDescent="0.3">
@@ -857,13 +870,13 @@
         <v>15</v>
       </c>
       <c r="B22" s="2" t="s">
-        <v>19</v>
+        <v>16</v>
       </c>
       <c r="C22" s="2">
-        <v>47</v>
+        <v>36</v>
       </c>
       <c r="D22" s="2">
-        <v>48</v>
+        <v>39</v>
       </c>
     </row>
     <row r="23" spans="1:4" x14ac:dyDescent="0.3">
@@ -871,68 +884,194 @@
         <v>15</v>
       </c>
       <c r="B23" s="2" t="s">
-        <v>20</v>
+        <v>17</v>
       </c>
       <c r="C23" s="2">
-        <v>50</v>
+        <v>39</v>
       </c>
       <c r="D23" s="2">
-        <v>51</v>
+        <v>42</v>
       </c>
     </row>
     <row r="24" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A24" s="2" t="s">
+      <c r="A24" s="3" t="s">
         <v>15</v>
       </c>
-      <c r="B24" s="2" t="s">
-        <v>21</v>
-      </c>
-      <c r="C24" s="2">
-        <v>51</v>
-      </c>
-      <c r="D24" s="2">
-        <v>55</v>
+      <c r="B24" s="3" t="s">
+        <v>38</v>
+      </c>
+      <c r="C24" s="3">
+        <v>42</v>
+      </c>
+      <c r="D24" s="3">
+        <v>44</v>
       </c>
     </row>
     <row r="25" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A25" s="2" t="s">
-        <v>22</v>
+        <v>15</v>
       </c>
       <c r="B25" s="2" t="s">
-        <v>30</v>
+        <v>18</v>
       </c>
       <c r="C25" s="2">
-        <v>59.2</v>
+        <v>44</v>
       </c>
       <c r="D25" s="2">
-        <v>61</v>
+        <v>45</v>
       </c>
     </row>
     <row r="26" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A26" s="2" t="s">
-        <v>22</v>
-      </c>
-      <c r="B26" s="2" t="s">
-        <v>23</v>
-      </c>
-      <c r="C26" s="2">
-        <v>63</v>
-      </c>
-      <c r="D26" s="2">
-        <v>64</v>
+      <c r="A26" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="B26" s="3" t="s">
+        <v>38</v>
+      </c>
+      <c r="C26" s="3">
+        <v>45</v>
+      </c>
+      <c r="D26" s="3">
+        <v>47</v>
       </c>
     </row>
     <row r="27" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A27" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="B27" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="C27" s="2">
+        <v>47</v>
+      </c>
+      <c r="D27" s="2">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="28" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A28" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="B28" s="3" t="s">
+        <v>38</v>
+      </c>
+      <c r="C28" s="3">
+        <v>48</v>
+      </c>
+      <c r="D28" s="3">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="29" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A29" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="B29" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="C29" s="2">
+        <v>50</v>
+      </c>
+      <c r="D29" s="2">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="30" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A30" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="B30" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="C30" s="2">
+        <v>51</v>
+      </c>
+      <c r="D30" s="2">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="31" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A31" s="3" t="s">
+        <v>39</v>
+      </c>
+      <c r="B31" s="3" t="s">
+        <v>38</v>
+      </c>
+      <c r="C31" s="3">
+        <v>55</v>
+      </c>
+      <c r="D31" s="3">
+        <v>59.2</v>
+      </c>
+    </row>
+    <row r="32" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A32" s="2" t="s">
         <v>22</v>
       </c>
-      <c r="B27" s="2" t="s">
+      <c r="B32" s="2" t="s">
+        <v>30</v>
+      </c>
+      <c r="C32" s="2">
+        <v>59.2</v>
+      </c>
+      <c r="D32" s="2">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="33" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A33" s="3" t="s">
+        <v>22</v>
+      </c>
+      <c r="B33" s="3" t="s">
+        <v>38</v>
+      </c>
+      <c r="C33" s="3">
+        <v>61</v>
+      </c>
+      <c r="D33" s="3">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="34" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A34" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="B34" s="2" t="s">
+        <v>23</v>
+      </c>
+      <c r="C34" s="2">
+        <v>63</v>
+      </c>
+      <c r="D34" s="2">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="35" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A35" s="3" t="s">
+        <v>22</v>
+      </c>
+      <c r="B35" s="3" t="s">
+        <v>38</v>
+      </c>
+      <c r="C35" s="3">
+        <v>64</v>
+      </c>
+      <c r="D35" s="3">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="36" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A36" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="B36" s="2" t="s">
         <v>24</v>
       </c>
-      <c r="C27" s="2">
+      <c r="C36" s="2">
         <v>65</v>
       </c>
-      <c r="D27" s="2">
+      <c r="D36" s="2">
         <v>66</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Correct typo on "Chapadmalan"
</commit_message>
<xml_diff>
--- a/data_2023/time_bins/SALMA.xlsx
+++ b/data_2023/time_bins/SALMA.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\Internship_ISEM\Neotropical_Mammals\REPO\Neotropical_mammals\data_2023\time_bins\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4A17516E-48F1-4C21-A38E-58778A843042}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{678A334D-51C8-463E-8760-80610785C5D9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28695" yWindow="0" windowWidth="14610" windowHeight="17385" xr2:uid="{04C64777-6055-495D-8002-BBD1BCB13666}"/>
+    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="17520" xr2:uid="{04C64777-6055-495D-8002-BBD1BCB13666}"/>
   </bookViews>
   <sheets>
     <sheet name="Feuil1" sheetId="1" r:id="rId1"/>
@@ -122,9 +122,6 @@
     <t>Tinguirirican</t>
   </si>
   <si>
-    <t>Chapadmalalan</t>
-  </si>
-  <si>
     <t>Mayoan</t>
   </si>
   <si>
@@ -174,6 +171,9 @@
   </si>
   <si>
     <t>Paleocene-Eocene</t>
+  </si>
+  <si>
+    <t>Chapadmalan</t>
   </si>
 </sst>
 </file>
@@ -563,7 +563,7 @@
   <dimension ref="A1:D36"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection sqref="A1:D36"/>
+      <selection activeCell="B7" sqref="B7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -573,10 +573,10 @@
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="B1" s="1" t="s">
         <v>31</v>
-      </c>
-      <c r="B1" s="1" t="s">
-        <v>32</v>
       </c>
       <c r="C1" s="1" t="s">
         <v>0</v>
@@ -587,10 +587,10 @@
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A2" s="2" t="s">
+        <v>33</v>
+      </c>
+      <c r="B2" s="2" t="s">
         <v>34</v>
-      </c>
-      <c r="B2" s="2" t="s">
-        <v>35</v>
       </c>
       <c r="C2" s="2">
         <v>0</v>
@@ -618,7 +618,7 @@
         <v>3</v>
       </c>
       <c r="B4" s="2" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="C4" s="2">
         <v>0.3</v>
@@ -643,7 +643,7 @@
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A6" s="2" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="B6" s="2" t="s">
         <v>26</v>
@@ -660,7 +660,7 @@
         <v>4</v>
       </c>
       <c r="B7" s="2" t="s">
-        <v>28</v>
+        <v>39</v>
       </c>
       <c r="C7" s="2">
         <v>3.3</v>
@@ -716,7 +716,7 @@
         <v>5</v>
       </c>
       <c r="B11" s="2" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="C11" s="2">
         <v>10</v>
@@ -758,7 +758,7 @@
         <v>5</v>
       </c>
       <c r="B14" s="2" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="C14" s="2">
         <v>15.5</v>
@@ -786,7 +786,7 @@
         <v>5</v>
       </c>
       <c r="B16" s="3" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="C16" s="3">
         <v>18</v>
@@ -814,7 +814,7 @@
         <v>5</v>
       </c>
       <c r="B18" s="3" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="C18" s="3">
         <v>21</v>
@@ -856,7 +856,7 @@
         <v>15</v>
       </c>
       <c r="B21" s="3" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="C21" s="3">
         <v>33.9</v>
@@ -898,7 +898,7 @@
         <v>15</v>
       </c>
       <c r="B24" s="3" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="C24" s="3">
         <v>42</v>
@@ -926,7 +926,7 @@
         <v>15</v>
       </c>
       <c r="B26" s="3" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="C26" s="3">
         <v>45</v>
@@ -954,7 +954,7 @@
         <v>15</v>
       </c>
       <c r="B28" s="3" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="C28" s="3">
         <v>48</v>
@@ -993,10 +993,10 @@
     </row>
     <row r="31" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A31" s="3" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="B31" s="3" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="C31" s="3">
         <v>55</v>
@@ -1010,7 +1010,7 @@
         <v>22</v>
       </c>
       <c r="B32" s="2" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="C32" s="2">
         <v>59.2</v>
@@ -1024,7 +1024,7 @@
         <v>22</v>
       </c>
       <c r="B33" s="3" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="C33" s="3">
         <v>61</v>
@@ -1052,7 +1052,7 @@
         <v>22</v>
       </c>
       <c r="B35" s="3" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="C35" s="3">
         <v>64</v>

</xml_diff>

<commit_message>
update SALMA in the case of the EOT
</commit_message>
<xml_diff>
--- a/data_2023/time_bins/SALMA.xlsx
+++ b/data_2023/time_bins/SALMA.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26327"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27029"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\Internship_ISEM\Neotropical_Mammals\REPO\Neotropical_mammals\data_2023\time_bins\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{678A334D-51C8-463E-8760-80610785C5D9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DBB43357-09AE-4030-8D31-274E5878A6F5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="17520" xr2:uid="{04C64777-6055-495D-8002-BBD1BCB13666}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{04C64777-6055-495D-8002-BBD1BCB13666}"/>
   </bookViews>
   <sheets>
     <sheet name="Feuil1" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="74" uniqueCount="40">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="95" uniqueCount="46">
   <si>
     <t>min_ma</t>
   </si>
@@ -175,12 +175,56 @@
   <si>
     <t>Chapadmalan</t>
   </si>
+  <si>
+    <t>Reference</t>
+  </si>
+  <si>
+    <t>La Cantera</t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">R. E. Dunn et al. (2013) A new chronology for middle Eocene-early Miocene South American Land Mammal ages. </t>
+    </r>
+    <r>
+      <rPr>
+        <i/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Geological Society of America Bulletin; 125, no. 3-4, 539-555.</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">M. O. Woodburne et al. (2013) Paleogene Land Mammal Faunas of South America; a Response to Global Climatic Changes and Indigenous Floral Diversity. </t>
+    </r>
+    <r>
+      <rPr>
+        <i/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Journal of Mammal Evolution. 21:1-73</t>
+    </r>
+  </si>
+  <si>
+    <t>Eocene-Oligocene</t>
+  </si>
+  <si>
+    <t>Oligocene-Miocene</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="4" x14ac:knownFonts="1">
+  <fonts count="5" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -204,6 +248,14 @@
     <font>
       <i/>
       <sz val="11"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <i/>
+      <sz val="11"/>
+      <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -560,10 +612,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{050431C4-1A0C-4966-AE29-90D56A8311BE}">
-  <dimension ref="A1:D36"/>
+  <dimension ref="A1:E41"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B7" sqref="B7"/>
+    <sheetView tabSelected="1" topLeftCell="A14" workbookViewId="0">
+      <selection activeCell="A19" sqref="A19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -571,7 +623,7 @@
     <col min="2" max="2" width="17.88671875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>30</v>
       </c>
@@ -584,8 +636,11 @@
       <c r="D1" s="1" t="s">
         <v>1</v>
       </c>
-    </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="E1" s="1" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A2" s="2" t="s">
         <v>33</v>
       </c>
@@ -599,7 +654,7 @@
         <v>1.17E-2</v>
       </c>
     </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A3" s="2" t="s">
         <v>3</v>
       </c>
@@ -613,7 +668,7 @@
         <v>0.3</v>
       </c>
     </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A4" s="2" t="s">
         <v>3</v>
       </c>
@@ -627,7 +682,7 @@
         <v>0.7</v>
       </c>
     </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A5" s="2" t="s">
         <v>3</v>
       </c>
@@ -641,7 +696,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A6" s="2" t="s">
         <v>36</v>
       </c>
@@ -655,7 +710,7 @@
         <v>3.3</v>
       </c>
     </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A7" s="2" t="s">
         <v>4</v>
       </c>
@@ -669,7 +724,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A8" s="2" t="s">
         <v>4</v>
       </c>
@@ -683,7 +738,7 @@
         <v>5.3330000000000002</v>
       </c>
     </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A9" s="2" t="s">
         <v>5</v>
       </c>
@@ -697,7 +752,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="10" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A10" s="2" t="s">
         <v>5</v>
       </c>
@@ -711,7 +766,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="11" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A11" s="2" t="s">
         <v>5</v>
       </c>
@@ -725,7 +780,7 @@
         <v>11.5</v>
       </c>
     </row>
-    <row r="12" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A12" s="2" t="s">
         <v>5</v>
       </c>
@@ -739,7 +794,7 @@
         <v>13.8</v>
       </c>
     </row>
-    <row r="13" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A13" s="2" t="s">
         <v>5</v>
       </c>
@@ -753,7 +808,7 @@
         <v>15.5</v>
       </c>
     </row>
-    <row r="14" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A14" s="2" t="s">
         <v>5</v>
       </c>
@@ -767,7 +822,7 @@
         <v>16.3</v>
       </c>
     </row>
-    <row r="15" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A15" s="2" t="s">
         <v>5</v>
       </c>
@@ -781,7 +836,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="16" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A16" s="3" t="s">
         <v>5</v>
       </c>
@@ -792,10 +847,10 @@
         <v>18</v>
       </c>
       <c r="D16" s="3">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="17" spans="1:4" x14ac:dyDescent="0.3">
+        <v>20.100000000000001</v>
+      </c>
+    </row>
+    <row r="17" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A17" s="2" t="s">
         <v>5</v>
       </c>
@@ -803,15 +858,18 @@
         <v>25</v>
       </c>
       <c r="C17" s="2">
-        <v>20</v>
+        <v>20.100000000000001</v>
       </c>
       <c r="D17" s="2">
         <v>21</v>
       </c>
-    </row>
-    <row r="18" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="E17" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="18" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A18" s="3" t="s">
-        <v>5</v>
+        <v>45</v>
       </c>
       <c r="B18" s="3" t="s">
         <v>37</v>
@@ -820,10 +878,10 @@
         <v>21</v>
       </c>
       <c r="D18" s="3">
-        <v>23.03</v>
-      </c>
-    </row>
-    <row r="19" spans="1:4" x14ac:dyDescent="0.3">
+        <v>24.2</v>
+      </c>
+    </row>
+    <row r="19" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A19" s="2" t="s">
         <v>13</v>
       </c>
@@ -831,97 +889,109 @@
         <v>14</v>
       </c>
       <c r="C19" s="2">
-        <v>23.03</v>
+        <v>24.2</v>
       </c>
       <c r="D19" s="2">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="20" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A20" s="2" t="s">
+        <v>29.4</v>
+      </c>
+      <c r="E19" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="20" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A20" s="3" t="s">
         <v>13</v>
       </c>
-      <c r="B20" s="2" t="s">
+      <c r="B20" s="3" t="s">
+        <v>37</v>
+      </c>
+      <c r="C20" s="3">
+        <v>29.4</v>
+      </c>
+      <c r="D20" s="3">
+        <v>30.617000000000001</v>
+      </c>
+    </row>
+    <row r="21" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A21" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="B21" s="2" t="s">
+        <v>41</v>
+      </c>
+      <c r="C21" s="2">
+        <v>30.617000000000001</v>
+      </c>
+      <c r="D21" s="2">
+        <v>30.77</v>
+      </c>
+      <c r="E21" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="22" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A22" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="B22" s="3" t="s">
+        <v>37</v>
+      </c>
+      <c r="C22" s="3">
+        <v>30.77</v>
+      </c>
+      <c r="D22" s="3">
+        <v>31.3</v>
+      </c>
+    </row>
+    <row r="23" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A23" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="B23" s="2" t="s">
         <v>27</v>
       </c>
-      <c r="C20" s="2">
-        <v>30</v>
-      </c>
-      <c r="D20" s="2">
-        <v>33.9</v>
-      </c>
-    </row>
-    <row r="21" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A21" s="3" t="s">
-        <v>15</v>
-      </c>
-      <c r="B21" s="3" t="s">
-        <v>37</v>
-      </c>
-      <c r="C21" s="3">
-        <v>33.9</v>
-      </c>
-      <c r="D21" s="3">
-        <v>36</v>
-      </c>
-    </row>
-    <row r="22" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A22" s="2" t="s">
-        <v>15</v>
-      </c>
-      <c r="B22" s="2" t="s">
-        <v>16</v>
-      </c>
-      <c r="C22" s="2">
-        <v>36</v>
-      </c>
-      <c r="D22" s="2">
-        <v>39</v>
-      </c>
-    </row>
-    <row r="23" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A23" s="2" t="s">
-        <v>15</v>
-      </c>
-      <c r="B23" s="2" t="s">
-        <v>17</v>
-      </c>
       <c r="C23" s="2">
-        <v>39</v>
+        <v>31.3</v>
       </c>
       <c r="D23" s="2">
+        <v>33.6</v>
+      </c>
+      <c r="E23" t="s">
         <v>42</v>
       </c>
     </row>
-    <row r="24" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A24" s="3" t="s">
-        <v>15</v>
+        <v>44</v>
       </c>
       <c r="B24" s="3" t="s">
         <v>37</v>
       </c>
       <c r="C24" s="3">
-        <v>42</v>
+        <v>33.6</v>
       </c>
       <c r="D24" s="3">
-        <v>44</v>
-      </c>
-    </row>
-    <row r="25" spans="1:4" x14ac:dyDescent="0.3">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="25" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A25" s="2" t="s">
         <v>15</v>
       </c>
       <c r="B25" s="2" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="C25" s="2">
-        <v>44</v>
+        <v>38</v>
       </c>
       <c r="D25" s="2">
-        <v>45</v>
-      </c>
-    </row>
-    <row r="26" spans="1:4" x14ac:dyDescent="0.3">
+        <v>38.200000000000003</v>
+      </c>
+      <c r="E25" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="26" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A26" s="3" t="s">
         <v>15</v>
       </c>
@@ -929,27 +999,30 @@
         <v>37</v>
       </c>
       <c r="C26" s="3">
-        <v>45</v>
+        <v>39</v>
       </c>
       <c r="D26" s="3">
-        <v>47</v>
-      </c>
-    </row>
-    <row r="27" spans="1:4" x14ac:dyDescent="0.3">
+        <v>38.200000000000003</v>
+      </c>
+    </row>
+    <row r="27" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A27" s="2" t="s">
         <v>15</v>
       </c>
       <c r="B27" s="2" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="C27" s="2">
-        <v>47</v>
+        <v>39</v>
       </c>
       <c r="D27" s="2">
-        <v>48</v>
-      </c>
-    </row>
-    <row r="28" spans="1:4" x14ac:dyDescent="0.3">
+        <v>41.7</v>
+      </c>
+      <c r="E27" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="28" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A28" s="3" t="s">
         <v>15</v>
       </c>
@@ -957,121 +1030,203 @@
         <v>37</v>
       </c>
       <c r="C28" s="3">
-        <v>48</v>
+        <v>41.7</v>
       </c>
       <c r="D28" s="3">
-        <v>50</v>
-      </c>
-    </row>
-    <row r="29" spans="1:4" x14ac:dyDescent="0.3">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="29" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A29" s="2" t="s">
         <v>15</v>
       </c>
       <c r="B29" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="C29" s="2">
+        <v>44</v>
+      </c>
+      <c r="D29" s="2">
+        <v>46</v>
+      </c>
+      <c r="E29" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="30" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A30" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="B30" s="3" t="s">
+        <v>37</v>
+      </c>
+      <c r="C30" s="3">
+        <v>46</v>
+      </c>
+      <c r="D30" s="3">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="31" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A31" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="B31" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="C31" s="2">
+        <v>47</v>
+      </c>
+      <c r="D31" s="2">
+        <v>49</v>
+      </c>
+      <c r="E31" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="32" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A32" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="B32" s="3" t="s">
+        <v>37</v>
+      </c>
+      <c r="C32" s="3">
+        <v>49</v>
+      </c>
+      <c r="D32" s="3">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="33" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A33" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="B33" s="2" t="s">
         <v>20</v>
       </c>
-      <c r="C29" s="2">
+      <c r="C33" s="2">
         <v>50</v>
       </c>
-      <c r="D29" s="2">
+      <c r="D33" s="2">
         <v>51</v>
       </c>
-    </row>
-    <row r="30" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A30" s="2" t="s">
+      <c r="E33" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="34" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A34" s="3" t="s">
         <v>15</v>
       </c>
-      <c r="B30" s="2" t="s">
+      <c r="B34" s="3" t="s">
+        <v>37</v>
+      </c>
+      <c r="C34" s="3">
+        <v>51</v>
+      </c>
+      <c r="D34" s="3">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="35" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A35" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="B35" s="2" t="s">
         <v>21</v>
       </c>
-      <c r="C30" s="2">
-        <v>51</v>
-      </c>
-      <c r="D30" s="2">
-        <v>55</v>
-      </c>
-    </row>
-    <row r="31" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A31" s="3" t="s">
+      <c r="C35" s="2">
+        <v>52</v>
+      </c>
+      <c r="D35" s="2">
+        <v>54</v>
+      </c>
+      <c r="E35" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="36" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A36" s="3" t="s">
         <v>38</v>
       </c>
-      <c r="B31" s="3" t="s">
+      <c r="B36" s="3" t="s">
         <v>37</v>
       </c>
-      <c r="C31" s="3">
-        <v>55</v>
-      </c>
-      <c r="D31" s="3">
+      <c r="C36" s="3">
+        <v>54</v>
+      </c>
+      <c r="D36" s="3">
         <v>59.2</v>
       </c>
     </row>
-    <row r="32" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A32" s="2" t="s">
+    <row r="37" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A37" s="2" t="s">
         <v>22</v>
       </c>
-      <c r="B32" s="2" t="s">
+      <c r="B37" s="2" t="s">
         <v>29</v>
       </c>
-      <c r="C32" s="2">
+      <c r="C37" s="2">
         <v>59.2</v>
       </c>
-      <c r="D32" s="2">
+      <c r="D37" s="2">
         <v>61</v>
       </c>
     </row>
-    <row r="33" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A33" s="3" t="s">
+    <row r="38" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A38" s="3" t="s">
         <v>22</v>
       </c>
-      <c r="B33" s="3" t="s">
+      <c r="B38" s="3" t="s">
         <v>37</v>
       </c>
-      <c r="C33" s="3">
+      <c r="C38" s="3">
         <v>61</v>
       </c>
-      <c r="D33" s="3">
+      <c r="D38" s="3">
         <v>63</v>
       </c>
     </row>
-    <row r="34" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A34" s="2" t="s">
+    <row r="39" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A39" s="2" t="s">
         <v>22</v>
       </c>
-      <c r="B34" s="2" t="s">
+      <c r="B39" s="2" t="s">
         <v>23</v>
       </c>
-      <c r="C34" s="2">
+      <c r="C39" s="2">
         <v>63</v>
       </c>
-      <c r="D34" s="2">
+      <c r="D39" s="2">
         <v>64</v>
       </c>
     </row>
-    <row r="35" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A35" s="3" t="s">
+    <row r="40" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A40" s="3" t="s">
         <v>22</v>
       </c>
-      <c r="B35" s="3" t="s">
+      <c r="B40" s="3" t="s">
         <v>37</v>
       </c>
-      <c r="C35" s="3">
+      <c r="C40" s="3">
         <v>64</v>
       </c>
-      <c r="D35" s="3">
+      <c r="D40" s="3">
         <v>65</v>
       </c>
     </row>
-    <row r="36" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A36" s="2" t="s">
+    <row r="41" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A41" s="2" t="s">
         <v>22</v>
       </c>
-      <c r="B36" s="2" t="s">
+      <c r="B41" s="2" t="s">
         <v>24</v>
       </c>
-      <c r="C36" s="2">
+      <c r="C41" s="2">
         <v>65</v>
       </c>
-      <c r="D36" s="2">
+      <c r="D41" s="2">
         <v>66</v>
       </c>
     </row>

</xml_diff>

<commit_message>
start tidying up this crazy repo
</commit_message>
<xml_diff>
--- a/data_2023/time_bins/SALMA.xlsx
+++ b/data_2023/time_bins/SALMA.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\Internship_ISEM\Neotropical_Mammals\REPO\Neotropical_mammals\data_2023\time_bins\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DBB43357-09AE-4030-8D31-274E5878A6F5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{93DE7E76-EE6C-4A99-9A17-FEB39E07E678}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{04C64777-6055-495D-8002-BBD1BCB13666}"/>
   </bookViews>
@@ -95,9 +95,6 @@
     <t>Vacan</t>
   </si>
   <si>
-    <t>Sapoan Fauna</t>
-  </si>
-  <si>
     <t>Riochican</t>
   </si>
   <si>
@@ -123,27 +120,6 @@
   </si>
   <si>
     <t>Mayoan</t>
-  </si>
-  <si>
-    <r>
-      <rPr>
-        <i/>
-        <sz val="11"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>Carodnia</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve"> Zone</t>
-    </r>
   </si>
   <si>
     <t>epoch</t>
@@ -218,6 +194,12 @@
   </si>
   <si>
     <t>Oligocene-Miocene</t>
+  </si>
+  <si>
+    <t>Carodnian</t>
+  </si>
+  <si>
+    <t>Sapoan</t>
   </si>
 </sst>
 </file>
@@ -293,11 +275,12 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -614,8 +597,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{050431C4-1A0C-4966-AE29-90D56A8311BE}">
   <dimension ref="A1:E41"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A14" workbookViewId="0">
-      <selection activeCell="A19" sqref="A19"/>
+    <sheetView tabSelected="1" topLeftCell="A17" workbookViewId="0">
+      <selection activeCell="B32" sqref="B32"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -625,10 +608,10 @@
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
       <c r="C1" s="1" t="s">
         <v>0</v>
@@ -637,15 +620,15 @@
         <v>1</v>
       </c>
       <c r="E1" s="1" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A2" s="2" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
       <c r="C2" s="2">
         <v>0</v>
@@ -673,7 +656,7 @@
         <v>3</v>
       </c>
       <c r="B4" s="2" t="s">
-        <v>32</v>
+        <v>30</v>
       </c>
       <c r="C4" s="2">
         <v>0.3</v>
@@ -698,10 +681,10 @@
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A6" s="2" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
       <c r="B6" s="2" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="C6" s="2">
         <v>1.8</v>
@@ -715,7 +698,7 @@
         <v>4</v>
       </c>
       <c r="B7" s="2" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="C7" s="2">
         <v>3.3</v>
@@ -771,7 +754,7 @@
         <v>5</v>
       </c>
       <c r="B11" s="2" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="C11" s="2">
         <v>10</v>
@@ -813,7 +796,7 @@
         <v>5</v>
       </c>
       <c r="B14" s="2" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
       <c r="C14" s="2">
         <v>15.5</v>
@@ -841,7 +824,7 @@
         <v>5</v>
       </c>
       <c r="B16" s="3" t="s">
-        <v>37</v>
+        <v>35</v>
       </c>
       <c r="C16" s="3">
         <v>18</v>
@@ -855,7 +838,7 @@
         <v>5</v>
       </c>
       <c r="B17" s="2" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="C17" s="2">
         <v>20.100000000000001</v>
@@ -864,15 +847,15 @@
         <v>21</v>
       </c>
       <c r="E17" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
     </row>
     <row r="18" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A18" s="3" t="s">
-        <v>45</v>
+        <v>43</v>
       </c>
       <c r="B18" s="3" t="s">
-        <v>37</v>
+        <v>35</v>
       </c>
       <c r="C18" s="3">
         <v>21</v>
@@ -895,7 +878,7 @@
         <v>29.4</v>
       </c>
       <c r="E19" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
     </row>
     <row r="20" spans="1:5" x14ac:dyDescent="0.3">
@@ -903,7 +886,7 @@
         <v>13</v>
       </c>
       <c r="B20" s="3" t="s">
-        <v>37</v>
+        <v>35</v>
       </c>
       <c r="C20" s="3">
         <v>29.4</v>
@@ -917,7 +900,7 @@
         <v>13</v>
       </c>
       <c r="B21" s="2" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
       <c r="C21" s="2">
         <v>30.617000000000001</v>
@@ -926,7 +909,7 @@
         <v>30.77</v>
       </c>
       <c r="E21" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
     </row>
     <row r="22" spans="1:5" x14ac:dyDescent="0.3">
@@ -934,7 +917,7 @@
         <v>13</v>
       </c>
       <c r="B22" s="3" t="s">
-        <v>37</v>
+        <v>35</v>
       </c>
       <c r="C22" s="3">
         <v>30.77</v>
@@ -948,7 +931,7 @@
         <v>13</v>
       </c>
       <c r="B23" s="2" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="C23" s="2">
         <v>31.3</v>
@@ -957,15 +940,15 @@
         <v>33.6</v>
       </c>
       <c r="E23" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
     </row>
     <row r="24" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A24" s="3" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
       <c r="B24" s="3" t="s">
-        <v>37</v>
+        <v>35</v>
       </c>
       <c r="C24" s="3">
         <v>33.6</v>
@@ -988,7 +971,7 @@
         <v>38.200000000000003</v>
       </c>
       <c r="E25" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
     </row>
     <row r="26" spans="1:5" x14ac:dyDescent="0.3">
@@ -996,7 +979,7 @@
         <v>15</v>
       </c>
       <c r="B26" s="3" t="s">
-        <v>37</v>
+        <v>35</v>
       </c>
       <c r="C26" s="3">
         <v>39</v>
@@ -1019,7 +1002,7 @@
         <v>41.7</v>
       </c>
       <c r="E27" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
     </row>
     <row r="28" spans="1:5" x14ac:dyDescent="0.3">
@@ -1027,7 +1010,7 @@
         <v>15</v>
       </c>
       <c r="B28" s="3" t="s">
-        <v>37</v>
+        <v>35</v>
       </c>
       <c r="C28" s="3">
         <v>41.7</v>
@@ -1050,7 +1033,7 @@
         <v>46</v>
       </c>
       <c r="E29" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
     </row>
     <row r="30" spans="1:5" x14ac:dyDescent="0.3">
@@ -1058,7 +1041,7 @@
         <v>15</v>
       </c>
       <c r="B30" s="3" t="s">
-        <v>37</v>
+        <v>35</v>
       </c>
       <c r="C30" s="3">
         <v>46</v>
@@ -1071,8 +1054,8 @@
       <c r="A31" s="2" t="s">
         <v>15</v>
       </c>
-      <c r="B31" s="2" t="s">
-        <v>19</v>
+      <c r="B31" s="4" t="s">
+        <v>45</v>
       </c>
       <c r="C31" s="2">
         <v>47</v>
@@ -1081,7 +1064,7 @@
         <v>49</v>
       </c>
       <c r="E31" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
     </row>
     <row r="32" spans="1:5" x14ac:dyDescent="0.3">
@@ -1089,7 +1072,7 @@
         <v>15</v>
       </c>
       <c r="B32" s="3" t="s">
-        <v>37</v>
+        <v>35</v>
       </c>
       <c r="C32" s="3">
         <v>49</v>
@@ -1103,7 +1086,7 @@
         <v>15</v>
       </c>
       <c r="B33" s="2" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="C33" s="2">
         <v>50</v>
@@ -1112,7 +1095,7 @@
         <v>51</v>
       </c>
       <c r="E33" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
     </row>
     <row r="34" spans="1:5" x14ac:dyDescent="0.3">
@@ -1120,7 +1103,7 @@
         <v>15</v>
       </c>
       <c r="B34" s="3" t="s">
-        <v>37</v>
+        <v>35</v>
       </c>
       <c r="C34" s="3">
         <v>51</v>
@@ -1134,7 +1117,7 @@
         <v>15</v>
       </c>
       <c r="B35" s="2" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="C35" s="2">
         <v>52</v>
@@ -1143,15 +1126,15 @@
         <v>54</v>
       </c>
       <c r="E35" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
     </row>
     <row r="36" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A36" s="3" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
       <c r="B36" s="3" t="s">
-        <v>37</v>
+        <v>35</v>
       </c>
       <c r="C36" s="3">
         <v>54</v>
@@ -1162,10 +1145,10 @@
     </row>
     <row r="37" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A37" s="2" t="s">
-        <v>22</v>
-      </c>
-      <c r="B37" s="2" t="s">
-        <v>29</v>
+        <v>21</v>
+      </c>
+      <c r="B37" s="4" t="s">
+        <v>44</v>
       </c>
       <c r="C37" s="2">
         <v>59.2</v>
@@ -1176,10 +1159,10 @@
     </row>
     <row r="38" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A38" s="3" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="B38" s="3" t="s">
-        <v>37</v>
+        <v>35</v>
       </c>
       <c r="C38" s="3">
         <v>61</v>
@@ -1190,10 +1173,10 @@
     </row>
     <row r="39" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A39" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="B39" s="2" t="s">
         <v>22</v>
-      </c>
-      <c r="B39" s="2" t="s">
-        <v>23</v>
       </c>
       <c r="C39" s="2">
         <v>63</v>
@@ -1204,10 +1187,10 @@
     </row>
     <row r="40" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A40" s="3" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="B40" s="3" t="s">
-        <v>37</v>
+        <v>35</v>
       </c>
       <c r="C40" s="3">
         <v>64</v>
@@ -1218,10 +1201,10 @@
     </row>
     <row r="41" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A41" s="2" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="B41" s="2" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="C41" s="2">
         <v>65</v>

</xml_diff>